<commit_message>
upates of esgf table
</commit_message>
<xml_diff>
--- a/esgf/euro-cordex-esgf.xlsx
+++ b/esgf/euro-cordex-esgf.xlsx
@@ -2461,7 +2461,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['clm', 'clwvi', 'clivi', 'cll', 'clh', 'va925', 'vas', 'ua925', 'uas', 'zg100', 'zg200', 'va700', 'va850', 'va100', 'va200', 'va300', 'va400', 'va500', 'va600', 'ua700', 'ua850', 'ua500', 'ua600', 'zg925', 'zmla', 'zg700', 'zg850', 'zg300', 'zg400', 'zg500', 'zg600', 'prw', 'rlut', 'mrros', 'mrso', 'mrfso', 'mrro', 'evspsbl', 'hus100', 'rsdt', 'rsut', 'hus850', 'hus925', 'hus200', 'hus300', 'hus400', 'hus500', 'hus600', 'hus700', 'snm', 'snw', 'snc', 'snd', 'ta925', 'ts', 'ua100', 'ua200', 'ua300', 'ua400', 'ta100', 'ta200', 'ta700', 'ta850', 'ta300', 'ta400', 'ta500', 'ta600']</t>
+          <t>['clm', 'clwvi', 'clivi', 'cll', 'clh', 'va925', 'vas', 'ua925', 'uas', 'zg100', 'zg200', 'va700', 'va850', 'va100', 'va200', 'va300', 'va400', 'va500', 'va600', 'ua700', 'ua850', 'ua500', 'ua600', 'zg925', 'zmla', 'zg700', 'zg850', 'zg300', 'zg400', 'zg500', 'zg600', 'snm', 'snw', 'snc', 'snd', 'ta925', 'ts', 'ua100', 'ua200', 'ua300', 'ua400', 'ta100', 'ta200', 'ta700', 'ta850', 'ta300', 'ta400', 'ta500', 'ta600', 'prw', 'rlut', 'mrros', 'mrso', 'mrfso', 'mrro', 'evspsbl', 'hus100', 'rsdt', 'rsut', 'hus850', 'hus925', 'hus200', 'hus300', 'hus400', 'hus500', 'hus600', 'hus700']</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>['evspsbl', 'hfls', 'hfss', 'hurs', 'hus100', 'clivi', 'cll', 'clm', 'clt', 'clwvi', 'mrro', 'mrros', 'mrso', 'pr', 'prc', 'hus700', 'hus850', 'hus925', 'huss', 'mrfso', 'hus200', 'hus300', 'hus400', 'hus500', 'hus600', 'clh', 'va850', 'va925', 'vas', 'wsgsmax', 'zg100', 'zg700', 'zg850', 'zg925', 'zmla', 'zg200', 'zg300', 'zg400', 'zg500', 'zg600', 'rlds', 'rlus', 'rlut', 'rsds', 'rsdt', 'prhmax', 'prsn', 'prw', 'ps', 'psl', 'snc', 'snd', 'snm', 'snw', 'sund', 'tasmax', 'tasmin', 'ts', 'ua100', 'ua200', 'ua850', 'ua925', 'uas', 'va100', 'va200', 'ta600', 'ta700', 'ta850', 'ta925', 'tas', 'ua300', 'ua400', 'ua500', 'ua600', 'ua700', 'ta100', 'ta200', 'ta300', 'ta400', 'ta500', 'rsus', 'rsut', 'sfcWind', 'sfcWindmax', 'va300', 'va400', 'va500', 'va600', 'va700']</t>
+          <t>['rlds', 'rlus', 'rlut', 'rsds', 'rsdt', 'prhmax', 'prsn', 'prw', 'ps', 'psl', 'snc', 'snd', 'snm', 'snw', 'sund', 'tasmax', 'tasmin', 'ts', 'ua100', 'ua200', 'ua850', 'ua925', 'uas', 'va100', 'va200', 'ta600', 'ta700', 'ta850', 'ta925', 'tas', 'ua300', 'ua400', 'ua500', 'ua600', 'ua700', 'ta100', 'ta200', 'ta300', 'ta400', 'ta500', 'rsus', 'rsut', 'sfcWind', 'sfcWindmax', 'evspsbl', 'hfls', 'hfss', 'hurs', 'hus100', 'clivi', 'cll', 'clm', 'clt', 'clwvi', 'mrro', 'mrros', 'mrso', 'pr', 'prc', 'hus700', 'hus850', 'hus925', 'huss', 'mrfso', 'hus200', 'hus300', 'hus400', 'hus500', 'hus600', 'clh', 'va300', 'va400', 'va500', 'va600', 'va700', 'va850', 'va925', 'vas', 'wsgsmax', 'zg100', 'zg700', 'zg850', 'zg925', 'zmla', 'zg200', 'zg300', 'zg400', 'zg500', 'zg600']</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>['rsdt', 'rsus', 'rsut', 'sfcWind', 'sfcWindmax', 'snc', 'pr', 'psl', 'rlds', 'rlus', 'rlut', 'rsds', 'evspsbl', 'hfls', 'hfss', 'hurs', 'hus100', 'hus200', 'hus925', 'huss', 'mrfso', 'mrro', 'mrros', 'mrso', 'hus300', 'hus400', 'hus500', 'hus600', 'hus700', 'hus850', 'clt', 'zg700', 'zg850', 'zg925', 'snd', 'snm', 'snw', 'sund', 'ta100', 'ta200', 'ta925', 'tas', 'tasmax', 'tasmin', 'ua100', 'ua200', 'ua925', 'uas', 'va100', 'va200', 'va300', 'va400', 'va500', 'va600', 'va700', 'va850', 'va925', 'vas', 'ua300', 'ua400', 'ua500', 'ua600', 'ua700', 'ua850', 'zg100', 'zg200', 'zg300', 'zg400', 'zg500', 'zg600', 'ta300', 'ta400', 'ta500', 'ta600', 'ta700', 'ta850']</t>
+          <t>['zg700', 'zg850', 'zg925', 'snd', 'snm', 'snw', 'sund', 'ta100', 'ta200', 'ta925', 'tas', 'tasmax', 'tasmin', 'ua100', 'ua200', 'ua925', 'uas', 'va100', 'va200', 'va300', 'va400', 'va500', 'va600', 'va700', 'va850', 'va925', 'vas', 'ua300', 'ua400', 'ua500', 'ua600', 'ua700', 'ua850', 'zg100', 'zg200', 'zg300', 'zg400', 'zg500', 'zg600', 'ta300', 'ta400', 'ta500', 'ta600', 'ta700', 'ta850', 'rsdt', 'rsus', 'rsut', 'sfcWind', 'sfcWindmax', 'snc', 'pr', 'psl', 'rlds', 'rlus', 'rlut', 'rsds', 'evspsbl', 'hfls', 'hfss', 'hurs', 'hus100', 'hus200', 'hus925', 'huss', 'mrfso', 'mrro', 'mrros', 'mrso', 'hus300', 'hus400', 'hus500', 'hus600', 'hus700', 'hus850', 'clt']</t>
         </is>
       </c>
     </row>

</xml_diff>